<commit_message>
Artemis example pipeline with Metadata template
</commit_message>
<xml_diff>
--- a/artemis/tools/Excel template/template.xlsx
+++ b/artemis/tools/Excel template/template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5880" windowHeight="8280"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="3090" windowHeight="7680" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset Info" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
   <si>
     <t>Dataset Metadata</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>Granularity Type</t>
+  </si>
+  <si>
+    <t>Synthetic Data Generator Name</t>
   </si>
 </sst>
 </file>
@@ -391,15 +394,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -409,9 +409,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -423,6 +420,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -438,16 +444,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -743,7 +749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
@@ -758,300 +764,300 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="19"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="20"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="21"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="16"/>
+      <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="5"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
-      <c r="B5" s="7" t="s">
+      <c r="A5" s="16"/>
+      <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
-      <c r="B6" s="7" t="s">
+      <c r="A6" s="16"/>
+      <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
-      <c r="B7" s="7" t="s">
+      <c r="A7" s="16"/>
+      <c r="B7" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
-      <c r="B8" s="7" t="s">
+      <c r="A8" s="16"/>
+      <c r="B8" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="23"/>
-      <c r="B9" s="7" t="s">
+      <c r="A9" s="16"/>
+      <c r="B9" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
-      <c r="B10" s="7" t="s">
+      <c r="A10" s="16"/>
+      <c r="B10" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="23"/>
-      <c r="B11" s="7" t="s">
+      <c r="A11" s="16"/>
+      <c r="B11" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="7" t="s">
+      <c r="A12" s="16"/>
+      <c r="B12" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="23"/>
-      <c r="B13" s="7" t="s">
+      <c r="A13" s="16"/>
+      <c r="B13" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
-      <c r="B15" s="7" t="s">
+      <c r="A15" s="16"/>
+      <c r="B15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="23"/>
-      <c r="B16" s="7" t="s">
+      <c r="A16" s="16"/>
+      <c r="B16" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
-      <c r="B17" s="7" t="s">
+      <c r="A17" s="16"/>
+      <c r="B17" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="24"/>
-      <c r="B18" s="8" t="s">
+      <c r="A18" s="17"/>
+      <c r="B18" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="23"/>
-      <c r="B20" s="7" t="s">
+      <c r="A20" s="16"/>
+      <c r="B20" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="23"/>
-      <c r="B21" s="7" t="s">
+      <c r="A21" s="16"/>
+      <c r="B21" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
-      <c r="B22" s="7" t="s">
+      <c r="A22" s="16"/>
+      <c r="B22" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="24"/>
-      <c r="B23" s="8" t="s">
+      <c r="A23" s="17"/>
+      <c r="B23" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
     </row>
     <row r="24" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="23"/>
-      <c r="B25" s="7" t="s">
+      <c r="A25" s="16"/>
+      <c r="B25" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
     </row>
     <row r="26" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="23"/>
-      <c r="B26" s="7" t="s">
+      <c r="A26" s="16"/>
+      <c r="B26" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
     </row>
     <row r="27" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="24"/>
-      <c r="B27" s="8" t="s">
+      <c r="A27" s="17"/>
+      <c r="B27" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
     </row>
     <row r="28" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
     </row>
     <row r="29" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="23"/>
-      <c r="B29" s="7" t="s">
+      <c r="A29" s="16"/>
+      <c r="B29" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
     </row>
     <row r="30" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
-      <c r="B30" s="7" t="s">
+      <c r="A30" s="16"/>
+      <c r="B30" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
     </row>
     <row r="31" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="23"/>
-      <c r="B31" s="7" t="s">
+      <c r="A31" s="16"/>
+      <c r="B31" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
     </row>
     <row r="32" spans="1:5" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="24"/>
-      <c r="B32" s="8" t="s">
+      <c r="A32" s="17"/>
+      <c r="B32" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1070,10 +1076,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1081,98 +1087,101 @@
     <col min="1" max="1" width="16.28515625" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
     <col min="3" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="10" width="16.28515625" customWidth="1"/>
-    <col min="11" max="11" width="31" customWidth="1"/>
-    <col min="12" max="12" width="32.7109375" customWidth="1"/>
-    <col min="13" max="14" width="9.140625" customWidth="1"/>
+    <col min="5" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="11" width="16.28515625" customWidth="1"/>
+    <col min="12" max="12" width="31" customWidth="1"/>
+    <col min="13" max="13" width="32.7109375" customWidth="1"/>
+    <col min="14" max="15" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="25"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="B1" s="23"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="M2" s="10" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="K3" s="14" t="s">
+      <c r="B3" s="3"/>
+      <c r="L3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="14" t="s">
+      <c r="M3" s="12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="4"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="K5" s="13" t="s">
+      <c r="B5" s="3"/>
+      <c r="L5" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="L5" s="13" t="s">
+      <c r="M5" s="11" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="J7" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="K7" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="K7" s="11"/>
+      <c r="L7" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>